<commit_message>
Calculus and vectors study
</commit_message>
<xml_diff>
--- a/6_Robotics/5_Vectors_Calculus/Calc-1.xlsx
+++ b/6_Robotics/5_Vectors_Calculus/Calc-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\6_Robotics\5_Vectors_Calculus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA709E1-BFBA-498A-9E0B-72EB9711E63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452C7225-B4DD-4CCD-8096-63122E794C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
     <t>f(x) = x^2</t>
   </si>
   <si>
-    <t>f'(x) = 2*x</t>
+    <t>f'(x) = f(x+dx)-f(x) / f(x)</t>
   </si>
 </sst>
 </file>
@@ -97,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -107,6 +107,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -254,32 +257,29 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1343,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D11"/>
+  <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1354,20 +1354,20 @@
     <col min="1" max="1" width="2.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.25" style="1" customWidth="1"/>
     <col min="5" max="7" width="9" style="1"/>
     <col min="8" max="8" width="11.125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" ht="36" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1376,25 +1376,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <f>B3^2</f>
+        <f t="shared" ref="C3:C12" si="0">B3^2</f>
         <v>1</v>
       </c>
-      <c r="D3" s="2">
-        <f>B3*2</f>
-        <v>2</v>
-      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <f>B4^2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D4" s="2">
-        <f>B4*2</f>
-        <v>4</v>
+        <f>C5-C4</f>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
@@ -1402,12 +1399,12 @@
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <f>B5^2</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="D5" s="2">
-        <f>B5*2</f>
-        <v>6</v>
+        <f>C6-C5</f>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
@@ -1415,12 +1412,12 @@
         <v>4</v>
       </c>
       <c r="C6" s="2">
-        <f>B6^2</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D6" s="2">
-        <f>B6*2</f>
-        <v>8</v>
+        <f>C7-C6</f>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
@@ -1428,12 +1425,12 @@
         <v>5</v>
       </c>
       <c r="C7" s="2">
-        <f>B7^2</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="D7" s="2">
-        <f>B7*2</f>
-        <v>10</v>
+        <f>C8-C7</f>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
@@ -1441,12 +1438,12 @@
         <v>6</v>
       </c>
       <c r="C8" s="2">
-        <f>B8^2</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="D8" s="2">
-        <f>B8*2</f>
-        <v>12</v>
+        <f>C9-C8</f>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
@@ -1454,12 +1451,12 @@
         <v>7</v>
       </c>
       <c r="C9" s="2">
-        <f>B9^2</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="D9" s="2">
-        <f>B9*2</f>
-        <v>14</v>
+        <f>C10-C9</f>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
@@ -1467,12 +1464,12 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <f>B10^2</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="D10" s="2">
-        <f>B10*2</f>
-        <v>16</v>
+        <f>C11-C10</f>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
@@ -1480,13 +1477,23 @@
         <v>9</v>
       </c>
       <c r="C11" s="2">
-        <f>B11^2</f>
+        <f t="shared" si="0"/>
         <v>81</v>
       </c>
       <c r="D11" s="2">
-        <f>B11*2</f>
-        <v>18</v>
-      </c>
+        <f>C12-C11</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>